<commit_message>
change the column name to Sample in example_data
</commit_message>
<xml_diff>
--- a/Example_data.xlsx
+++ b/Example_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sviatoslavkharuk/Documents/WorkDepartment/KBB_PCR/Github-Analysis-of-qRT-PCR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sviatoslavkharuk/Documents/WorkDepartment/KBB_PCR/Github-Analysis-of-qRT-PCR/Analysis-of-qRT-PCR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D523D2-4FCC-8946-A572-EF9B279EC391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9071D44-A00D-6E4C-A7D9-9B930B867617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7706342F-EBA3-4C00-88DC-ADD53BADD20A}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>Target</t>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>Ct</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>RR</t>
+  </si>
+  <si>
+    <t>Sample</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -432,13 +432,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -446,7 +446,7 @@
         <v>414</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>29.2</v>
@@ -457,7 +457,7 @@
         <v>415</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>28.15</v>
@@ -468,7 +468,7 @@
         <v>417</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>27.49</v>
@@ -479,7 +479,7 @@
         <v>418</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>27.16</v>
@@ -490,7 +490,7 @@
         <v>414</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>26.78</v>
@@ -501,7 +501,7 @@
         <v>415</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>26.3</v>
@@ -512,7 +512,7 @@
         <v>417</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>25.73</v>
@@ -523,7 +523,7 @@
         <v>418</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>25.58</v>
@@ -534,7 +534,7 @@
         <v>414</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>25.32</v>
@@ -545,7 +545,7 @@
         <v>415</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>25.28</v>
@@ -556,7 +556,7 @@
         <v>417</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>25.23</v>
@@ -567,7 +567,7 @@
         <v>418</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>25.18</v>
@@ -578,7 +578,7 @@
         <v>428</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>25.16</v>
@@ -589,7 +589,7 @@
         <v>430</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>25</v>
@@ -600,7 +600,7 @@
         <v>431</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>24.98</v>
@@ -611,7 +611,7 @@
         <v>432</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>24.91</v>
@@ -622,7 +622,7 @@
         <v>428</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>24.85</v>
@@ -633,7 +633,7 @@
         <v>430</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>24.85</v>
@@ -644,7 +644,7 @@
         <v>431</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>24.83</v>
@@ -655,7 +655,7 @@
         <v>432</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>24.81</v>
@@ -666,7 +666,7 @@
         <v>428</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>24.74</v>
@@ -677,7 +677,7 @@
         <v>430</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>24.73</v>
@@ -688,7 +688,7 @@
         <v>431</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>24.63</v>
@@ -699,7 +699,7 @@
         <v>432</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <v>24.55</v>
@@ -710,7 +710,7 @@
         <v>483</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>24.53</v>
@@ -721,7 +721,7 @@
         <v>484</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>24.44</v>
@@ -732,7 +732,7 @@
         <v>485</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <v>24.39</v>
@@ -743,7 +743,7 @@
         <v>486</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>24.37</v>
@@ -754,7 +754,7 @@
         <v>483</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>24.35</v>
@@ -765,7 +765,7 @@
         <v>484</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>24.28</v>
@@ -776,7 +776,7 @@
         <v>485</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32">
         <v>24.17</v>
@@ -787,7 +787,7 @@
         <v>486</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33">
         <v>24</v>
@@ -798,7 +798,7 @@
         <v>483</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34">
         <v>23.88</v>
@@ -809,7 +809,7 @@
         <v>484</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35">
         <v>23.85</v>
@@ -820,7 +820,7 @@
         <v>485</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36">
         <v>23.77</v>
@@ -831,7 +831,7 @@
         <v>486</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>23.57</v>
@@ -842,7 +842,7 @@
         <v>423</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38">
         <v>22.22</v>
@@ -853,7 +853,7 @@
         <v>424</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39">
         <v>22.12</v>
@@ -864,7 +864,7 @@
         <v>426</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <v>22.07</v>
@@ -875,7 +875,7 @@
         <v>427</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>21.99</v>
@@ -886,7 +886,7 @@
         <v>423</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42">
         <v>21.87</v>
@@ -897,7 +897,7 @@
         <v>424</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43">
         <v>21.81</v>
@@ -908,7 +908,7 @@
         <v>426</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44">
         <v>21.78</v>
@@ -919,7 +919,7 @@
         <v>427</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45">
         <v>21.73</v>
@@ -930,7 +930,7 @@
         <v>423</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>21.71</v>
@@ -941,7 +941,7 @@
         <v>424</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>21.65</v>
@@ -952,7 +952,7 @@
         <v>426</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>21.65</v>
@@ -963,7 +963,7 @@
         <v>427</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>21.65</v>
@@ -974,7 +974,7 @@
         <v>414</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50">
         <v>20.95</v>
@@ -985,7 +985,7 @@
         <v>415</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51">
         <v>20.93</v>
@@ -996,7 +996,7 @@
         <v>417</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52">
         <v>20.48</v>
@@ -1007,7 +1007,7 @@
         <v>418</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53">
         <v>20.329999999999998</v>
@@ -1018,7 +1018,7 @@
         <v>414</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54">
         <v>20.13</v>
@@ -1029,7 +1029,7 @@
         <v>415</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C55">
         <v>19.940000000000001</v>
@@ -1040,7 +1040,7 @@
         <v>417</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56">
         <v>19.920000000000002</v>
@@ -1051,7 +1051,7 @@
         <v>418</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C57">
         <v>19.760000000000002</v>
@@ -1062,7 +1062,7 @@
         <v>414</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C58">
         <v>19.75</v>
@@ -1073,7 +1073,7 @@
         <v>415</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C59">
         <v>19.71</v>
@@ -1084,7 +1084,7 @@
         <v>417</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C60">
         <v>19.7</v>
@@ -1095,7 +1095,7 @@
         <v>418</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C61">
         <v>19.66</v>
@@ -1106,7 +1106,7 @@
         <v>428</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62">
         <v>19.649999999999999</v>
@@ -1117,7 +1117,7 @@
         <v>430</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63">
         <v>19.62</v>
@@ -1128,7 +1128,7 @@
         <v>431</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64">
         <v>19.54</v>
@@ -1139,7 +1139,7 @@
         <v>432</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65">
         <v>19.489999999999998</v>
@@ -1150,7 +1150,7 @@
         <v>428</v>
       </c>
       <c r="B66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C66">
         <v>19.440000000000001</v>
@@ -1161,7 +1161,7 @@
         <v>430</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C67">
         <v>19.39</v>
@@ -1172,7 +1172,7 @@
         <v>431</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C68">
         <v>19.079999999999998</v>
@@ -1183,7 +1183,7 @@
         <v>432</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C69">
         <v>19.07</v>
@@ -1194,7 +1194,7 @@
         <v>428</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C70">
         <v>19.02</v>
@@ -1205,7 +1205,7 @@
         <v>430</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C71">
         <v>19</v>
@@ -1216,7 +1216,7 @@
         <v>431</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C72">
         <v>18.98</v>
@@ -1227,7 +1227,7 @@
         <v>432</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C73">
         <v>18.97</v>
@@ -1238,7 +1238,7 @@
         <v>483</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C74">
         <v>18.95</v>
@@ -1249,7 +1249,7 @@
         <v>484</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C75">
         <v>18.940000000000001</v>
@@ -1260,7 +1260,7 @@
         <v>485</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76">
         <v>18.93</v>
@@ -1271,7 +1271,7 @@
         <v>486</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77">
         <v>18.93</v>
@@ -1282,7 +1282,7 @@
         <v>483</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C78">
         <v>18.53</v>
@@ -1293,7 +1293,7 @@
         <v>484</v>
       </c>
       <c r="B79" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C79">
         <v>18.440000000000001</v>
@@ -1304,7 +1304,7 @@
         <v>485</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C80">
         <v>18.440000000000001</v>
@@ -1315,7 +1315,7 @@
         <v>486</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C81">
         <v>18.37</v>
@@ -1326,7 +1326,7 @@
         <v>483</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C82">
         <v>18.36</v>
@@ -1337,7 +1337,7 @@
         <v>484</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C83">
         <v>18.36</v>
@@ -1348,7 +1348,7 @@
         <v>485</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C84">
         <v>18.27</v>
@@ -1359,7 +1359,7 @@
         <v>486</v>
       </c>
       <c r="B85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C85">
         <v>18.21</v>
@@ -1370,7 +1370,7 @@
         <v>423</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C86">
         <v>18.21</v>
@@ -1381,7 +1381,7 @@
         <v>424</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C87">
         <v>18.13</v>
@@ -1392,7 +1392,7 @@
         <v>426</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C88">
         <v>18.03</v>
@@ -1403,7 +1403,7 @@
         <v>427</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C89">
         <v>18.010000000000002</v>
@@ -1414,7 +1414,7 @@
         <v>423</v>
       </c>
       <c r="B90" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C90">
         <v>17.98</v>
@@ -1425,7 +1425,7 @@
         <v>424</v>
       </c>
       <c r="B91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C91">
         <v>17.940000000000001</v>
@@ -1436,7 +1436,7 @@
         <v>426</v>
       </c>
       <c r="B92" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C92">
         <v>17.809999999999999</v>
@@ -1447,7 +1447,7 @@
         <v>427</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C93">
         <v>17.27</v>
@@ -1458,7 +1458,7 @@
         <v>423</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C94">
         <v>17.27</v>
@@ -1469,7 +1469,7 @@
         <v>424</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C95">
         <v>17.13</v>
@@ -1480,7 +1480,7 @@
         <v>426</v>
       </c>
       <c r="B96" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C96">
         <v>16.940000000000001</v>
@@ -1491,7 +1491,7 @@
         <v>427</v>
       </c>
       <c r="B97" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C97">
         <v>16.59</v>

</xml_diff>